<commit_message>
sửa lại tính năng đối soat
</commit_message>
<xml_diff>
--- a/public/files/import/Doi_soat_ghtk (1).xlsx
+++ b/public/files/import/Doi_soat_ghtk (1).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34E3555-D9E9-4AF6-968E-DE6ECE162C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252B5A65-F5DF-45FC-AB49-5D852384791B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,19 +179,19 @@
  </t>
   </si>
   <si>
-    <t>S14075533.HN66-E4.1419414334---1</t>
-  </si>
-  <si>
-    <t>S14075533.MB9-16-B1.1097600185--11</t>
-  </si>
-  <si>
-    <t>S14075533.MB9-04-B6.1267956153-111</t>
-  </si>
-  <si>
-    <t>S14075533.MB3-06-G25.1721880608--111</t>
-  </si>
-  <si>
-    <t>S14075533.MB25-30-R21.1350325011-111</t>
+    <t>S14075533.HN66-E4.1419414334</t>
+  </si>
+  <si>
+    <t>S14075533.MB9-16-B1.1097600185</t>
+  </si>
+  <si>
+    <t>S14075533.MB9-04-B6.1267956153</t>
+  </si>
+  <si>
+    <t>S14075533.MB3-06-G25.1721880608</t>
+  </si>
+  <si>
+    <t>S14075533.MB25-30-R21.1350325011</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>